<commit_message>
modified tagging script, beging delete tags
</commit_message>
<xml_diff>
--- a/python_examples/uuid_tagging/uuidTags.xlsx
+++ b/python_examples/uuid_tagging/uuidTags.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.sullivan/APIS/API_scripts/api-examples/python_examples/uuidTagging/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.sullivan/APIS/API_scripts/api-examples/python_examples/uuid_tagging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B41BF-84F4-D348-9527-CDAAC83717B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB0D500-6B04-9647-89D7-3C538E0ABA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="820" windowWidth="26020" windowHeight="15200" xr2:uid="{FF299712-7879-A446-A8AD-05C2FA114891}"/>
+    <workbookView xWindow="11120" yWindow="820" windowWidth="26020" windowHeight="15200" xr2:uid="{FF299712-7879-A446-A8AD-05C2FA114891}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Tags</t>
   </si>
@@ -44,22 +44,118 @@
     <t>company ID</t>
   </si>
   <si>
-    <t>UUID</t>
-  </si>
-  <si>
-    <t>tag1</t>
-  </si>
-  <si>
-    <t>tag2</t>
-  </si>
-  <si>
-    <t>tag3</t>
-  </si>
-  <si>
-    <t>tag4</t>
-  </si>
-  <si>
-    <t>tag5</t>
+    <t>794f77ff-2f0c-4179-a4a2-73860c12bdb7</t>
+  </si>
+  <si>
+    <t>a6a4f9d6-324c-453c-8b78-671c47eb415e</t>
+  </si>
+  <si>
+    <t>6176b7a7-0e42-4c13-a808-e61325eb38d2</t>
+  </si>
+  <si>
+    <t>fd11a23d-beec-4fa9-a7bf-2e4356ce1ac9</t>
+  </si>
+  <si>
+    <t>425a2b55-f4fb-4650-831f-a3675be0bebc</t>
+  </si>
+  <si>
+    <t>78938f6a-b07b-4a49-872a-f7a94c34895d</t>
+  </si>
+  <si>
+    <t>3c753432-2b49-43c8-91fb-ac4c96833886</t>
+  </si>
+  <si>
+    <t>4d7639ce-41fa-41be-b215-43f69d7f258b</t>
+  </si>
+  <si>
+    <t>3f6c5c45-2d48-4760-b7e7-9c59fd1512b1</t>
+  </si>
+  <si>
+    <t>d14f5a3e-249f-49db-89de-ca258bcecaf7</t>
+  </si>
+  <si>
+    <t>a2b1c956-6104-44dd-b22f-beee0526d24f</t>
+  </si>
+  <si>
+    <t>2aedfdd8-afc0-4d94-a92f-0d2a9fb5507e</t>
+  </si>
+  <si>
+    <t>c5edcc52-480a-440f-97cd-50aac4e9fbef</t>
+  </si>
+  <si>
+    <t>1b4ec6d8-ddb4-44ab-9dc6-307b64e97500</t>
+  </si>
+  <si>
+    <t>25bdb23c-1188-4541-a0fb-8288ab886315</t>
+  </si>
+  <si>
+    <t>3c324c2b-6b14-4816-88c2-02582ecc7d4a</t>
+  </si>
+  <si>
+    <t>8704ee68-341b-454a-bec3-f11a06da4b32</t>
+  </si>
+  <si>
+    <t>742c663a-2b15-4145-8f3e-01a45ea2188c</t>
+  </si>
+  <si>
+    <t>dabf5dab-da4f-40ff-81f2-96f267c3829b</t>
+  </si>
+  <si>
+    <t>tag, test, comp1</t>
+  </si>
+  <si>
+    <t>tag, test, comp2</t>
+  </si>
+  <si>
+    <t>tag, test, comp3</t>
+  </si>
+  <si>
+    <t>tag, test, comp4</t>
+  </si>
+  <si>
+    <t>tag, test, comp5</t>
+  </si>
+  <si>
+    <t>tag, test, comp6</t>
+  </si>
+  <si>
+    <t>tag, test, comp7</t>
+  </si>
+  <si>
+    <t>tag, test, comp8</t>
+  </si>
+  <si>
+    <t>tag, test, comp9</t>
+  </si>
+  <si>
+    <t>tag, test, comp10</t>
+  </si>
+  <si>
+    <t>tag, test, comp11</t>
+  </si>
+  <si>
+    <t>tag, test, comp12</t>
+  </si>
+  <si>
+    <t>tag, test, comp13</t>
+  </si>
+  <si>
+    <t>tag, test, comp14</t>
+  </si>
+  <si>
+    <t>tag, test, comp15</t>
+  </si>
+  <si>
+    <t>tag, test, comp16</t>
+  </si>
+  <si>
+    <t>tag, test, comp17</t>
+  </si>
+  <si>
+    <t>tag, test, comp18</t>
+  </si>
+  <si>
+    <t>tag, test, comp19</t>
   </si>
 </sst>
 </file>
@@ -417,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC30B05-F15F-E146-867B-581909F39FE2}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,39 +538,151 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>